<commit_message>
Modificacion generar desde PDF a PDF, MEJOR CALIDAD
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/ejemplo.xlsx
+++ b/src/main/resources/assets/ejemplo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joser\OneDrive\Documents\MisCodigos\DiplomaPDF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joser\OneDrive\Documents\MisCodigos\DiplomaPDF\src\main\resources\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,31 +24,172 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>José Ramón</t>
-  </si>
-  <si>
-    <t>Ainara Lahuerta</t>
-  </si>
-  <si>
-    <t>Ignacio Vela</t>
-  </si>
-  <si>
-    <t>Helena Vizcay</t>
-  </si>
-  <si>
-    <t>Ciro Artigot</t>
-  </si>
-  <si>
-    <t>Lucia Dalmau</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+  <si>
+    <t>José Ramón Gimeno Aguirregomozcorta</t>
+  </si>
+  <si>
+    <t>Ainara Lahuerta Cuartero</t>
+  </si>
+  <si>
+    <t>Helena Vizcay Goñi</t>
+  </si>
+  <si>
+    <t>Víctor Viñuales Edo</t>
+  </si>
+  <si>
+    <t>María Oria Almudi</t>
+  </si>
+  <si>
+    <t>Pablo Barrenechea Abecia</t>
+  </si>
+  <si>
+    <t>Ninoska de la Cruz Aráuz Hernández</t>
+  </si>
+  <si>
+    <t>María Ofelia Arteaga</t>
+  </si>
+  <si>
+    <t>Ciro Artigot Cordero</t>
+  </si>
+  <si>
+    <t>Charles Castro Lampón</t>
+  </si>
+  <si>
+    <t>Leire Díez Alzueta</t>
+  </si>
+  <si>
+    <t>Cecilia Foronda Diez</t>
+  </si>
+  <si>
+    <t>Eva González Lasheras</t>
+  </si>
+  <si>
+    <t>Magdalena del Carmen Hernández Delgado</t>
+  </si>
+  <si>
+    <t>Charo Romero Pérez</t>
+  </si>
+  <si>
+    <t>Carlos Martínez Castillo</t>
+  </si>
+  <si>
+    <t>Ana Lapeña Laiglesia</t>
+  </si>
+  <si>
+    <t>Ana Mastral Gascón de Gotor</t>
+  </si>
+  <si>
+    <t>Diane McAndrew</t>
+  </si>
+  <si>
+    <t>Ana Pérez Munárriz</t>
+  </si>
+  <si>
+    <t>Carlos Pesqué Castillo</t>
+  </si>
+  <si>
+    <t>Cuca Ramos Moreno</t>
+  </si>
+  <si>
+    <t>Aranzazu Romero Baigorri</t>
+  </si>
+  <si>
+    <t>Rafael Rubio de Val</t>
+  </si>
+  <si>
+    <t>Inocencia del Carmen Rugama Delgadillo</t>
+  </si>
+  <si>
+    <t>Marina Judith Guerrero Martínez</t>
+  </si>
+  <si>
+    <t>Mª Jesús Sanz Sanjoaquín</t>
+  </si>
+  <si>
+    <t>Patricia Tejero Toribio</t>
+  </si>
+  <si>
+    <t>Cristian Quílez Salete</t>
+  </si>
+  <si>
+    <t>Alejandra Gimeno  Aguirregomozcorta</t>
+  </si>
+  <si>
+    <t>Daniel Sanz Martínez</t>
+  </si>
+  <si>
+    <t>Mario Rodríguez Vargas</t>
+  </si>
+  <si>
+    <t>Lucía Dalmau Menéndez</t>
+  </si>
+  <si>
+    <t>Marcos Boj Pérez</t>
+  </si>
+  <si>
+    <t>Javier Tobías González</t>
+  </si>
+  <si>
+    <t>Jeannette Bain</t>
+  </si>
+  <si>
+    <t>Nacho Vela Gómez</t>
+  </si>
+  <si>
+    <t>Jon Moreno Oliva</t>
+  </si>
+  <si>
+    <t>Raquel Gonzalo Gómez</t>
+  </si>
+  <si>
+    <t>Vanessa Amigot Zardoya</t>
+  </si>
+  <si>
+    <t>Asun Santesteban García</t>
+  </si>
+  <si>
+    <t>Leyre Vallés Arbeloa</t>
+  </si>
+  <si>
+    <t>Javier Monterde Serrano</t>
+  </si>
+  <si>
+    <t>Nicolás Grassa López</t>
+  </si>
+  <si>
+    <t>Philippine Ménager</t>
+  </si>
+  <si>
+    <t>Silvia Tudela Aguilar</t>
+  </si>
+  <si>
+    <t>Elvira Boza Samanes</t>
+  </si>
+  <si>
+    <t>Cristina Sarregui Álvarez</t>
+  </si>
+  <si>
+    <t>Lola Berna Gascón</t>
+  </si>
+  <si>
+    <t>Nicole Julien</t>
+  </si>
+  <si>
+    <t>María Trinidad Meavilla Baquedano</t>
+  </si>
+  <si>
+    <t>Linda Lizeth Ramos Ramos</t>
+  </si>
+  <si>
+    <t>Blanca Oehling Durán</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +204,38 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,14 +255,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -368,49 +552,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/29-maria-oria-almudi"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/10-pablo-barrenechea"/>
+    <hyperlink ref="A5" r:id="rId3" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/15-maria-ofelia-arteaga"/>
+    <hyperlink ref="A6" r:id="rId4" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/16-ciro-artigot-cordero"/>
+    <hyperlink ref="A7" r:id="rId5" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/17-charles-castro-lampon"/>
+    <hyperlink ref="A8" r:id="rId6" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/18-leire-diez-alzueta"/>
+    <hyperlink ref="A9" r:id="rId7" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/19-cecilia-foronda-diez"/>
+    <hyperlink ref="A10" r:id="rId8" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/21-eva-gonzalez-lasheras"/>
+    <hyperlink ref="A11" r:id="rId9" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/22-carmela-hernandez-delgado"/>
+    <hyperlink ref="A12" r:id="rId10" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/34-charo-romero"/>
+    <hyperlink ref="A13" r:id="rId11" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/24-carlos-martinez"/>
+    <hyperlink ref="A14" r:id="rId12" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/23-ana-lapena-laiglesia"/>
+    <hyperlink ref="A15" r:id="rId13" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/26-ana-mastral-gascon-de-gotor"/>
+    <hyperlink ref="A16" r:id="rId14" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/27-diane-mcandrew"/>
+    <hyperlink ref="A17" r:id="rId15" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/30-ana-perez-munarriz"/>
+    <hyperlink ref="A18" r:id="rId16" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/31-carlos-pesque"/>
+    <hyperlink ref="A19" r:id="rId17" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/32-cuca-ramos-moreno"/>
+    <hyperlink ref="A20" r:id="rId18" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/35-aranzazu-romero-baigorri"/>
+    <hyperlink ref="A21" r:id="rId19" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/36-rafael-rubio-de-val"/>
+    <hyperlink ref="A22" r:id="rId20" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/37-inocencia-del-carmen-rugama-delgadillo"/>
+    <hyperlink ref="A24" r:id="rId21" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/39-m-jesus-sanz-sanjoaquin"/>
+    <hyperlink ref="A26" r:id="rId22" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/47-cristian-quilez"/>
+    <hyperlink ref="A28" r:id="rId23" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/81-helena-vizcay"/>
+    <hyperlink ref="A29" r:id="rId24" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/86-daniel-sanz"/>
+    <hyperlink ref="A30" r:id="rId25" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/87-mario-rodriguez-vargas"/>
+    <hyperlink ref="A31" r:id="rId26" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/88-lucia-dalmau-menendez"/>
+    <hyperlink ref="A32" r:id="rId27" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/89-marcos-boj-perez"/>
+    <hyperlink ref="A33" r:id="rId28" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/91-javier-tobias-gonzalez"/>
+    <hyperlink ref="A34" r:id="rId29" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/92-jose-ramon-gimeno"/>
+    <hyperlink ref="A35" r:id="rId30" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/93-jeannette-bain"/>
+    <hyperlink ref="A36" r:id="rId31" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/94-ainara-lahuerta"/>
+    <hyperlink ref="A37" r:id="rId32" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/95-nacho-vela"/>
+    <hyperlink ref="A38" r:id="rId33" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/96-jon-moreno-oliva"/>
+    <hyperlink ref="A39" r:id="rId34" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/97-raquel-gonzalo"/>
+    <hyperlink ref="A40" r:id="rId35" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/98-vanessa-amigot"/>
+    <hyperlink ref="A41" r:id="rId36" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/99-asun-santesteban"/>
+    <hyperlink ref="A42" r:id="rId37" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/102-leyre-valles-arbeloa"/>
+    <hyperlink ref="A43" r:id="rId38" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/103-javier-monterde"/>
+    <hyperlink ref="A44" r:id="rId39" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/104-nicolas-grassa"/>
+    <hyperlink ref="A45" r:id="rId40" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/105-philippine-menager"/>
+    <hyperlink ref="A46" r:id="rId41" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/106-silvia-tudela"/>
+    <hyperlink ref="A47" r:id="rId42" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/108-elvira-boza"/>
+    <hyperlink ref="A48" r:id="rId43" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/109-cristina-sarregui"/>
+    <hyperlink ref="A49" r:id="rId44" display="https://ecodes.org/quienes-somos/equipo/equipo-de-trabajo/110-lola-berna"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>